<commit_message>
Update CPIT380-Group Project - Rubric(1).xlsx
</commit_message>
<xml_diff>
--- a/CPIT380-Group Project - Rubric(1).xlsx
+++ b/CPIT380-Group Project - Rubric(1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nero\Documents\NetBeansProjects\Cpit380_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nero\Documents\GitHub\Cpit380Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321094B8-C883-481E-B702-29AE368EEFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254CD210-E5F6-46AA-BD53-0808C3C4D223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="67">
   <si>
     <r>
       <t>S</t>
@@ -459,12 +459,6 @@
     <t>Counting Number of Vehicles - User will input an  video where some vehicles will pass through and system will count how many vehicles are present in that image or video. User may use toy cars.</t>
   </si>
   <si>
-    <t xml:space="preserve">make it dsplay in the gui </t>
-  </si>
-  <si>
-    <t>fix gui</t>
-  </si>
-  <si>
     <t>Tracking Method - User will input a video and detect an object, frame by frame and continue drawing rectangle in each frame to track the object e.g. a flying bird in the video may be tracked or moving vehicle. Than save the video</t>
   </si>
   <si>
@@ -474,13 +468,7 @@
     <t>need to train the open cv</t>
   </si>
   <si>
-    <t xml:space="preserve">make it dsplay in the gui only work with face need to train the open cv to detact opject </t>
-  </si>
-  <si>
-    <t>its correct but nah</t>
-  </si>
-  <si>
-    <t>need to change the code</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -575,7 +563,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -590,12 +578,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -603,12 +585,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -765,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -854,94 +830,79 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1260,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,13 +1239,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="282.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1331,9 +1292,7 @@
       <c r="E3" s="17">
         <v>0</v>
       </c>
-      <c r="F3" s="18">
-        <v>2</v>
-      </c>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
@@ -1351,9 +1310,7 @@
       <c r="E4" s="17">
         <v>1</v>
       </c>
-      <c r="F4" s="18">
-        <v>1</v>
-      </c>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
@@ -1503,7 +1460,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D12" s="16">
         <v>1</v>
@@ -1521,7 +1478,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D13" s="16">
         <v>2</v>
@@ -1539,7 +1496,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D14" s="16">
         <v>3</v>
@@ -1612,15 +1569,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>16</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="20" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D18" s="22">
         <v>0</v>
@@ -1652,24 +1609,22 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="38">
+      <c r="A20" s="34">
         <v>18</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="35">
+      <c r="C20" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="31">
         <v>3</v>
       </c>
-      <c r="E20" s="36">
+      <c r="E20" s="32">
         <v>3</v>
       </c>
-      <c r="F20" s="37" t="s">
-        <v>70</v>
-      </c>
+      <c r="F20" s="33"/>
       <c r="G20" s="10">
         <v>3</v>
       </c>
@@ -1724,7 +1679,7 @@
         <v>29</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D23" s="22">
         <v>3</v>
@@ -1798,24 +1753,22 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="42">
+      <c r="A27" s="13">
         <v>25</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="35">
+      <c r="C27" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="22">
         <v>0</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="23">
         <v>0</v>
       </c>
-      <c r="F27" s="37" t="s">
-        <v>63</v>
-      </c>
+      <c r="F27" s="24"/>
     </row>
     <row r="28" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
@@ -1866,13 +1819,13 @@
       <c r="B30" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="40">
-        <v>2</v>
-      </c>
-      <c r="E30" s="41">
+      <c r="C30" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="36">
+        <v>2</v>
+      </c>
+      <c r="E30" s="37">
         <v>1</v>
       </c>
       <c r="F30" s="24"/>
@@ -1986,24 +1939,22 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="49">
+      <c r="A36" s="13">
         <v>35</v>
       </c>
-      <c r="B36" s="54" t="s">
+      <c r="B36" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="55">
+      <c r="C36" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="22">
         <v>5</v>
       </c>
-      <c r="E36" s="47">
+      <c r="E36" s="23">
         <v>4</v>
       </c>
-      <c r="F36" s="48" t="s">
-        <v>69</v>
-      </c>
+      <c r="F36" s="24"/>
       <c r="I36" s="10">
         <v>4</v>
       </c>
@@ -2177,44 +2128,40 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="42">
+      <c r="A45" s="13">
         <v>45</v>
       </c>
-      <c r="B45" s="59" t="s">
+      <c r="B45" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="35">
+      <c r="C45" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="22">
         <v>0</v>
       </c>
-      <c r="E45" s="36">
+      <c r="E45" s="23">
         <v>0</v>
       </c>
-      <c r="F45" s="37" t="s">
-        <v>64</v>
-      </c>
+      <c r="F45" s="24"/>
     </row>
     <row r="46" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="38">
+      <c r="A46" s="19">
         <v>46</v>
       </c>
-      <c r="B46" s="43" t="s">
+      <c r="B46" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="35">
+      <c r="C46" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="22">
         <v>5</v>
       </c>
-      <c r="E46" s="36">
+      <c r="E46" s="23">
         <v>0</v>
       </c>
-      <c r="F46" s="37" t="s">
-        <v>64</v>
-      </c>
+      <c r="F46" s="24"/>
     </row>
     <row r="47" spans="1:9" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
@@ -2238,71 +2185,71 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="38">
+      <c r="A48" s="19">
         <v>48</v>
       </c>
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="22">
+        <v>0</v>
+      </c>
+      <c r="E48" s="23">
+        <v>0</v>
+      </c>
+      <c r="F48" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="42">
+        <v>49</v>
+      </c>
+      <c r="B49" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="35">
+      <c r="D49" s="39">
         <v>0</v>
       </c>
-      <c r="E48" s="36">
+      <c r="E49" s="40">
         <v>0</v>
       </c>
-      <c r="F48" s="37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="49">
-        <v>49</v>
-      </c>
-      <c r="B49" s="32" t="s">
+      <c r="F49" s="41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="43">
+        <v>50</v>
+      </c>
+      <c r="B50" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="45">
+        <v>0</v>
+      </c>
+      <c r="E50" s="46">
+        <v>0</v>
+      </c>
+      <c r="F50" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="D49" s="46">
-        <v>0</v>
-      </c>
-      <c r="E49" s="47">
-        <v>0</v>
-      </c>
-      <c r="F49" s="48" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="50">
-        <v>50</v>
-      </c>
-      <c r="B50" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C50" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="D50" s="52">
-        <v>0</v>
-      </c>
-      <c r="E50" s="53">
-        <v>0</v>
-      </c>
-      <c r="F50" s="48" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="58" t="s">
+      <c r="A51" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="58"/>
-      <c r="C51" s="58"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
       <c r="D51" s="6">
         <f>SUM(D3:D50)</f>
         <v>100</v>
@@ -2313,7 +2260,7 @@
       </c>
       <c r="F51" s="6">
         <f>SUM(F3:F50)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G51" s="6">
         <f t="shared" ref="G51:I51" si="0">SUM(G3:G50)</f>
@@ -2329,11 +2276,11 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="58" t="s">
+      <c r="A52" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="58"/>
-      <c r="C52" s="58"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
       <c r="D52" s="12">
         <v>20</v>
       </c>
@@ -2348,10 +2295,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C53" s="58"/>
+      <c r="C53" s="49"/>
       <c r="D53" s="12">
         <v>5</v>
       </c>
@@ -2363,10 +2310,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
-      <c r="B54" s="58" t="s">
+      <c r="B54" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="58"/>
+      <c r="C54" s="49"/>
       <c r="D54" s="12">
         <v>25</v>
       </c>

</xml_diff>